<commit_message>
fix import users, survey expires
</commit_message>
<xml_diff>
--- a/src/assets/template/user-import-template.xlsx
+++ b/src/assets/template/user-import-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972A51FA-D099-534F-ABE7-2AD4DC498D20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B95BF75-BEC7-7A4B-9482-3C68F462AB2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="2200" windowWidth="20740" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>fullName</t>
   </si>
@@ -31,36 +31,6 @@
     <t>phone</t>
   </si>
   <si>
-    <t>@hoidanit1</t>
-  </si>
-  <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>@hoidanit2</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>@hoidanit3</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>@hoidanit4</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
-  </si>
-  <si>
-    <t>@hoidanit5</t>
-  </si>
-  <si>
-    <t>test5@gmail.com</t>
-  </si>
-  <si>
     <t>christianName</t>
   </si>
   <si>
@@ -70,23 +40,74 @@
     <t>0765482765</t>
   </si>
   <si>
-    <t>0765482766</t>
-  </si>
-  <si>
-    <t>0765482767</t>
-  </si>
-  <si>
-    <t>0765482768</t>
-  </si>
-  <si>
-    <t>0765482769</t>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>fatherName</t>
+  </si>
+  <si>
+    <t>fatherPhone</t>
+  </si>
+  <si>
+    <t>motherName</t>
+  </si>
+  <si>
+    <t>motherPhone</t>
+  </si>
+  <si>
+    <t>parish</t>
+  </si>
+  <si>
+    <t>deanery</t>
+  </si>
+  <si>
+    <t>spiritualDirectorName</t>
+  </si>
+  <si>
+    <t>sponsoringPriestName</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>Nguyen Minh</t>
+  </si>
+  <si>
+    <t>Xuan Loc</t>
+  </si>
+  <si>
+    <t>testchoi@gmail.com</t>
+  </si>
+  <si>
+    <t>12-12-2003</t>
+  </si>
+  <si>
+    <t>Nguyen Van B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,6 +146,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,18 +176,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,10 +409,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -386,11 +420,13 @@
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -401,76 +437,105 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>